<commit_message>
Editting consumption value input to include elec only/gas only OFGEM MEDIUM archetypes, some further formatting modification to marketgrid.xlsx
</commit_message>
<xml_diff>
--- a/Raw Data/Consumption Values.xlsx
+++ b/Raw Data/Consumption Values.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Archetype</t>
   </si>
@@ -151,6 +151,21 @@
   </si>
   <si>
     <t>Gareth's tropical mansion</t>
+  </si>
+  <si>
+    <t>Single Fuel</t>
+  </si>
+  <si>
+    <t>OFGEM: MEDIUM (E-ONLY)</t>
+  </si>
+  <si>
+    <t>OFGEM: MEDIUM (G-ONLY)</t>
+  </si>
+  <si>
+    <t>OfgemMedE</t>
+  </si>
+  <si>
+    <t>OfgemMedG</t>
   </si>
 </sst>
 </file>
@@ -335,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -378,15 +393,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -446,6 +452,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -835,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,31 +868,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34"/>
-      <c r="B1" s="26" t="s">
+      <c r="A1" s="31"/>
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="19" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="23.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="36" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -897,7 +918,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
@@ -921,7 +942,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
@@ -945,7 +966,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
@@ -969,7 +990,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="34.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -995,7 +1016,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1019,7 +1040,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
@@ -1043,7 +1064,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1067,7 +1088,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
@@ -1091,7 +1112,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1115,7 +1136,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
@@ -1139,7 +1160,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1163,23 +1184,23 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="23" t="s">
+      <c r="A14" s="32"/>
+      <c r="B14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="21">
         <v>24531000</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="22">
         <v>1</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="21">
         <v>4378</v>
       </c>
-      <c r="F14" s="24">
+      <c r="F14" s="21">
         <v>17100</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="26">
         <v>1281</v>
       </c>
       <c r="H14" t="s">
@@ -1187,23 +1208,23 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="19">
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="16">
         <f>'[1]Results (tables)'!D5</f>
         <v>2000</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="16">
         <f>'[1]Results (tables)'!D8</f>
         <v>9000</v>
       </c>
-      <c r="G15" s="30">
+      <c r="G15" s="27">
         <f>'[1]Results (tables)'!D11</f>
         <v>877.5962833333333</v>
       </c>
@@ -1212,7 +1233,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="11" t="s">
         <v>23</v>
       </c>
@@ -1235,21 +1256,21 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18" t="s">
+      <c r="A17" s="38"/>
+      <c r="B17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="19">
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="16">
         <f>'[1]Results (tables)'!D7</f>
         <v>4900</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="16">
         <f>'[1]Results (tables)'!D10</f>
         <v>19000</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="18">
         <f>'[1]Results (tables)'!D13</f>
         <v>1758.3806458333333</v>
       </c>
@@ -1258,31 +1279,72 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="37">
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="34">
         <v>7931</v>
       </c>
-      <c r="F18" s="37">
+      <c r="F18" s="34">
         <v>47856</v>
       </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="38" t="s">
+      <c r="G18" s="30"/>
+      <c r="H18" s="35" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="34">
+        <f>E16</f>
+        <v>3200</v>
+      </c>
+      <c r="F19" s="34">
+        <v>0</v>
+      </c>
+      <c r="G19" s="30"/>
+      <c r="H19" s="35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="39"/>
+      <c r="B20" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="34">
+        <v>0</v>
+      </c>
+      <c r="F20" s="34">
+        <f>F16</f>
+        <v>13500</v>
+      </c>
+      <c r="G20" s="30"/>
+      <c r="H20" s="35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A13"/>
     <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A19:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>